<commit_message>
updated annoatations and input file
</commit_message>
<xml_diff>
--- a/input/Input_7_17_2020.xlsx
+++ b/input/Input_7_17_2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aeast\OneDrive - Environmental Protection Agency (EPA)\Profile\Desktop\LEM4\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A38F66-009D-469E-8470-DE6344BE99A7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB5DC28-DBF4-4CEF-94C6-B4ED01FC88B1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4140" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{954D9476-CD18-4396-BAEA-D273523A90CB}"/>
+    <workbookView xWindow="28680" yWindow="-4140" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{954D9476-CD18-4396-BAEA-D273523A90CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="8" r:id="rId1"/>
@@ -583,9 +583,6 @@
     <t>Happonen, M., et al. (2016). "Contamination risk ofrawdrinking water caused by PFOA sources along a river reach in south-western Finland"</t>
   </si>
   <si>
-    <t>Groudnwater</t>
-  </si>
-  <si>
     <t>South-western</t>
   </si>
   <si>
@@ -1481,6 +1478,9 @@
   </si>
   <si>
     <t>PFOA PFOS Intake Model Input File</t>
+  </si>
+  <si>
+    <t>Groundwater</t>
   </si>
 </sst>
 </file>
@@ -1956,7 +1956,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A1" s="10" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1964,52 +1964,52 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -2029,7 +2029,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -2072,66 +2072,66 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="S1" s="8" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B2">
         <v>200</v>
@@ -2177,7 +2177,7 @@
         <v>13</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Q2" s="9">
         <v>0.9</v>
@@ -2191,7 +2191,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -2237,7 +2237,7 @@
         <v>71.3</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="Q3" s="9">
         <v>0.9</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B4">
         <v>200</v>
@@ -2297,7 +2297,7 @@
         <v>60</v>
       </c>
       <c r="P4" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q4" s="9">
         <v>0.9</v>
@@ -2318,7 +2318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C8F63D-B204-4F59-8FB9-7A9F72E511A1}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -2334,10 +2334,10 @@
         <v>5</v>
       </c>
       <c r="B1" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="C1" s="17" t="s">
         <v>271</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2371,8 +2371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1616EC2E-64FD-472E-8B72-98A928CE2F2B}">
   <dimension ref="A1:AT142"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AT141" sqref="AT141"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2403,13 +2403,13 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -2543,22 +2543,22 @@
         <v>48</v>
       </c>
       <c r="K2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L2">
         <v>39</v>
       </c>
       <c r="M2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N2">
         <v>2570</v>
       </c>
       <c r="O2" t="s">
+        <v>285</v>
+      </c>
+      <c r="P2" t="s">
         <v>286</v>
-      </c>
-      <c r="P2" t="s">
-        <v>287</v>
       </c>
       <c r="R2">
         <v>28</v>
@@ -2647,7 +2647,7 @@
         <v>4</v>
       </c>
       <c r="K3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L3">
         <v>39</v>
@@ -2695,7 +2695,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L4">
         <v>20</v>
@@ -2708,10 +2708,10 @@
         <v>400</v>
       </c>
       <c r="O4" t="s">
+        <v>287</v>
+      </c>
+      <c r="P4" t="s">
         <v>288</v>
-      </c>
-      <c r="P4" t="s">
-        <v>289</v>
       </c>
       <c r="Z4" t="s">
         <v>57</v>
@@ -2800,7 +2800,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L5">
         <v>20</v>
@@ -2813,10 +2813,10 @@
         <v>440</v>
       </c>
       <c r="O5" t="s">
+        <v>289</v>
+      </c>
+      <c r="P5" t="s">
         <v>290</v>
-      </c>
-      <c r="P5" t="s">
-        <v>291</v>
       </c>
       <c r="Z5" t="s">
         <v>57</v>
@@ -2899,22 +2899,22 @@
         <v>56</v>
       </c>
       <c r="K6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L6">
         <v>12</v>
       </c>
       <c r="M6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="N6">
         <v>89</v>
       </c>
       <c r="O6" t="s">
+        <v>292</v>
+      </c>
+      <c r="P6" t="s">
         <v>293</v>
-      </c>
-      <c r="P6" t="s">
-        <v>294</v>
       </c>
       <c r="Z6" t="s">
         <v>57</v>
@@ -3003,7 +3003,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L7">
         <v>12</v>
@@ -3016,10 +3016,10 @@
         <v>200</v>
       </c>
       <c r="O7" t="s">
+        <v>294</v>
+      </c>
+      <c r="P7" t="s">
         <v>295</v>
-      </c>
-      <c r="P7" t="s">
-        <v>296</v>
       </c>
       <c r="Z7" t="s">
         <v>57</v>
@@ -3108,7 +3108,7 @@
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L8">
         <v>57</v>
@@ -3121,10 +3121,10 @@
         <v>2.93</v>
       </c>
       <c r="O8" t="s">
+        <v>296</v>
+      </c>
+      <c r="P8" t="s">
         <v>297</v>
-      </c>
-      <c r="P8" t="s">
-        <v>298</v>
       </c>
       <c r="Q8">
         <v>0.51</v>
@@ -3216,7 +3216,7 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L9">
         <v>57</v>
@@ -3229,10 +3229,10 @@
         <v>5.04</v>
       </c>
       <c r="O9" t="s">
+        <v>298</v>
+      </c>
+      <c r="P9" t="s">
         <v>299</v>
-      </c>
-      <c r="P9" t="s">
-        <v>300</v>
       </c>
       <c r="Q9">
         <v>0.89</v>
@@ -3324,7 +3324,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L10">
         <v>57</v>
@@ -3337,10 +3337,10 @@
         <v>99.8</v>
       </c>
       <c r="O10" t="s">
+        <v>300</v>
+      </c>
+      <c r="P10" t="s">
         <v>301</v>
-      </c>
-      <c r="P10" t="s">
-        <v>302</v>
       </c>
       <c r="Q10">
         <v>18</v>
@@ -3426,13 +3426,13 @@
         <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I11">
         <v>0.2</v>
       </c>
       <c r="K11" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L11">
         <v>57</v>
@@ -3475,7 +3475,7 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L12">
         <v>6</v>
@@ -3488,7 +3488,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="P12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Z12" t="s">
         <v>49</v>
@@ -3574,7 +3574,7 @@
         <v>4</v>
       </c>
       <c r="K13" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L13">
         <v>6</v>
@@ -3586,7 +3586,7 @@
         <v>1.3333333333333299E-2</v>
       </c>
       <c r="O13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P13">
         <v>1.3333333333333299E-2</v>
@@ -3675,7 +3675,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L14">
         <v>10</v>
@@ -3688,7 +3688,7 @@
         <v>6.1</v>
       </c>
       <c r="O14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P14">
         <v>2.2999999999999998</v>
@@ -3777,7 +3777,7 @@
         <v>76</v>
       </c>
       <c r="K15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L15">
         <v>10</v>
@@ -3790,10 +3790,10 @@
         <v>20</v>
       </c>
       <c r="O15" t="s">
+        <v>306</v>
+      </c>
+      <c r="P15" t="s">
         <v>307</v>
-      </c>
-      <c r="P15" t="s">
-        <v>308</v>
       </c>
       <c r="Z15" t="s">
         <v>57</v>
@@ -3879,7 +3879,7 @@
         <v>78</v>
       </c>
       <c r="K16" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L16">
         <v>16</v>
@@ -3968,13 +3968,13 @@
         <v>82</v>
       </c>
       <c r="K17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L17">
         <v>16</v>
       </c>
       <c r="P17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Z17" t="s">
         <v>79</v>
@@ -4057,13 +4057,13 @@
         <v>78</v>
       </c>
       <c r="K18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L18">
         <v>12</v>
       </c>
       <c r="P18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z18" t="s">
         <v>83</v>
@@ -4146,13 +4146,13 @@
         <v>82</v>
       </c>
       <c r="K19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L19">
         <v>12</v>
       </c>
       <c r="P19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z19" t="s">
         <v>83</v>
@@ -4247,7 +4247,7 @@
         <v>1390</v>
       </c>
       <c r="O20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P20">
         <v>97</v>
@@ -4348,7 +4348,7 @@
         <v>4661</v>
       </c>
       <c r="O21" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P21">
         <v>280</v>
@@ -4519,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="AT22" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:46" x14ac:dyDescent="0.3">
@@ -5073,16 +5073,16 @@
         <v>20</v>
       </c>
       <c r="M28" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N28">
         <v>1500</v>
       </c>
       <c r="O28" t="s">
+        <v>314</v>
+      </c>
+      <c r="P28" t="s">
         <v>315</v>
-      </c>
-      <c r="P28" t="s">
-        <v>316</v>
       </c>
       <c r="Z28" t="s">
         <v>57</v>
@@ -5181,10 +5181,10 @@
         <v>370</v>
       </c>
       <c r="O29" t="s">
+        <v>316</v>
+      </c>
+      <c r="P29" t="s">
         <v>317</v>
-      </c>
-      <c r="P29" t="s">
-        <v>318</v>
       </c>
       <c r="Z29" t="s">
         <v>57</v>
@@ -5270,16 +5270,16 @@
         <v>42</v>
       </c>
       <c r="M30" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="N30">
         <v>3700</v>
       </c>
       <c r="O30" t="s">
+        <v>319</v>
+      </c>
+      <c r="P30" t="s">
         <v>320</v>
-      </c>
-      <c r="P30" t="s">
-        <v>321</v>
       </c>
       <c r="Z30" t="s">
         <v>57</v>
@@ -5371,16 +5371,16 @@
         <v>42</v>
       </c>
       <c r="M31" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N31">
         <v>1700</v>
       </c>
       <c r="O31" t="s">
+        <v>321</v>
+      </c>
+      <c r="P31" t="s">
         <v>322</v>
-      </c>
-      <c r="P31" t="s">
-        <v>323</v>
       </c>
       <c r="Z31" t="s">
         <v>57</v>
@@ -5466,16 +5466,16 @@
         <v>45</v>
       </c>
       <c r="M32" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N32">
         <v>7400</v>
       </c>
       <c r="O32" t="s">
+        <v>323</v>
+      </c>
+      <c r="P32" t="s">
         <v>324</v>
-      </c>
-      <c r="P32" t="s">
-        <v>325</v>
       </c>
       <c r="Z32" t="s">
         <v>57</v>
@@ -5574,10 +5574,10 @@
         <v>4100</v>
       </c>
       <c r="O33" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P33" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Z33" t="s">
         <v>57</v>
@@ -5663,16 +5663,16 @@
         <v>20</v>
       </c>
       <c r="M34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N34">
         <v>1000</v>
       </c>
       <c r="O34" t="s">
+        <v>326</v>
+      </c>
+      <c r="P34" t="s">
         <v>327</v>
-      </c>
-      <c r="P34" t="s">
-        <v>328</v>
       </c>
       <c r="Z34" t="s">
         <v>57</v>
@@ -5771,10 +5771,10 @@
         <v>6000</v>
       </c>
       <c r="O35" t="s">
+        <v>328</v>
+      </c>
+      <c r="P35" t="s">
         <v>329</v>
-      </c>
-      <c r="P35" t="s">
-        <v>330</v>
       </c>
       <c r="Z35" t="s">
         <v>57</v>
@@ -5936,16 +5936,16 @@
         <v>19</v>
       </c>
       <c r="M38" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="N38">
         <v>1300</v>
       </c>
       <c r="O38" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P38" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Z38" t="s">
         <v>105</v>
@@ -6044,10 +6044,10 @@
         <v>4000</v>
       </c>
       <c r="O39" t="s">
+        <v>331</v>
+      </c>
+      <c r="P39" t="s">
         <v>332</v>
-      </c>
-      <c r="P39" t="s">
-        <v>333</v>
       </c>
       <c r="Z39" t="s">
         <v>105</v>
@@ -6133,16 +6133,16 @@
         <v>10</v>
       </c>
       <c r="M40" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N40">
         <v>1700</v>
       </c>
       <c r="O40" t="s">
+        <v>334</v>
+      </c>
+      <c r="P40" t="s">
         <v>335</v>
-      </c>
-      <c r="P40" t="s">
-        <v>336</v>
       </c>
       <c r="Z40" t="s">
         <v>106</v>
@@ -6228,16 +6228,16 @@
         <v>10</v>
       </c>
       <c r="M41" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="N41">
         <v>220</v>
       </c>
       <c r="O41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="P41" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="Z41" t="s">
         <v>106</v>
@@ -6323,16 +6323,16 @@
         <v>10</v>
       </c>
       <c r="M42" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="N42">
         <v>1000</v>
       </c>
       <c r="O42" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P42" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Z42" t="s">
         <v>108</v>
@@ -6418,16 +6418,16 @@
         <v>10</v>
       </c>
       <c r="M43" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="N43">
         <v>730</v>
       </c>
       <c r="O43" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="P43" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Z43" t="s">
         <v>108</v>
@@ -6513,16 +6513,16 @@
         <v>10</v>
       </c>
       <c r="M44" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N44">
         <v>930</v>
       </c>
       <c r="O44" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="Z44" t="s">
         <v>110</v>
@@ -6611,16 +6611,16 @@
         <v>10</v>
       </c>
       <c r="M45" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="N45">
         <v>1800</v>
       </c>
       <c r="O45" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="P45" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Z45" t="s">
         <v>110</v>
@@ -6899,10 +6899,10 @@
         <v>26.7</v>
       </c>
       <c r="O50" t="s">
+        <v>344</v>
+      </c>
+      <c r="P50" t="s">
         <v>345</v>
-      </c>
-      <c r="P50" t="s">
-        <v>346</v>
       </c>
       <c r="Z50" t="s">
         <v>114</v>
@@ -6962,7 +6962,7 @@
         <v>0</v>
       </c>
       <c r="AT50" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="51" spans="1:46" x14ac:dyDescent="0.3">
@@ -7007,10 +7007,10 @@
         <v>118</v>
       </c>
       <c r="O51" t="s">
+        <v>347</v>
+      </c>
+      <c r="P51" t="s">
         <v>348</v>
-      </c>
-      <c r="P51" t="s">
-        <v>349</v>
       </c>
       <c r="Z51" t="s">
         <v>114</v>
@@ -7093,7 +7093,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="H52" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I52" t="s">
         <v>113</v>
@@ -7105,16 +7105,16 @@
         <v>20</v>
       </c>
       <c r="M52" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="N52">
         <v>92.7</v>
       </c>
       <c r="O52" t="s">
+        <v>351</v>
+      </c>
+      <c r="P52" t="s">
         <v>352</v>
-      </c>
-      <c r="P52" t="s">
-        <v>353</v>
       </c>
       <c r="Z52" t="s">
         <v>105</v>
@@ -7206,16 +7206,16 @@
         <v>20</v>
       </c>
       <c r="M53" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N53">
         <v>31.8</v>
       </c>
       <c r="O53" t="s">
+        <v>354</v>
+      </c>
+      <c r="P53" t="s">
         <v>355</v>
-      </c>
-      <c r="P53" t="s">
-        <v>356</v>
       </c>
       <c r="Z53" t="s">
         <v>105</v>
@@ -7317,10 +7317,10 @@
         <v>318</v>
       </c>
       <c r="O54" t="s">
+        <v>356</v>
+      </c>
+      <c r="P54" t="s">
         <v>357</v>
-      </c>
-      <c r="P54" t="s">
-        <v>358</v>
       </c>
       <c r="Z54" t="s">
         <v>119</v>
@@ -7415,16 +7415,16 @@
         <v>20</v>
       </c>
       <c r="M55" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N55">
         <v>239</v>
       </c>
       <c r="O55" t="s">
+        <v>359</v>
+      </c>
+      <c r="P55" t="s">
         <v>360</v>
-      </c>
-      <c r="P55" t="s">
-        <v>361</v>
       </c>
       <c r="Z55" t="s">
         <v>119</v>
@@ -7526,10 +7526,10 @@
         <v>310</v>
       </c>
       <c r="O56" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="P56" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="Z56" t="s">
         <v>122</v>
@@ -7618,16 +7618,16 @@
         <v>10</v>
       </c>
       <c r="M57" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="N57">
         <v>699</v>
       </c>
       <c r="O57" t="s">
+        <v>363</v>
+      </c>
+      <c r="P57" t="s">
         <v>364</v>
-      </c>
-      <c r="P57" t="s">
-        <v>365</v>
       </c>
       <c r="Z57" t="s">
         <v>122</v>
@@ -7726,10 +7726,10 @@
         <v>192</v>
       </c>
       <c r="O58" t="s">
+        <v>365</v>
+      </c>
+      <c r="P58" t="s">
         <v>366</v>
-      </c>
-      <c r="P58" t="s">
-        <v>367</v>
       </c>
       <c r="Z58" t="s">
         <v>124</v>
@@ -7818,16 +7818,16 @@
         <v>10</v>
       </c>
       <c r="M59" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="N59">
         <v>149</v>
       </c>
       <c r="O59" t="s">
+        <v>368</v>
+      </c>
+      <c r="P59" t="s">
         <v>369</v>
-      </c>
-      <c r="P59" t="s">
-        <v>370</v>
       </c>
       <c r="Z59" t="s">
         <v>124</v>
@@ -7926,10 +7926,10 @@
         <v>129</v>
       </c>
       <c r="O60" t="s">
+        <v>370</v>
+      </c>
+      <c r="P60" t="s">
         <v>371</v>
-      </c>
-      <c r="P60" t="s">
-        <v>372</v>
       </c>
       <c r="Z60" t="s">
         <v>126</v>
@@ -8018,16 +8018,16 @@
         <v>7</v>
       </c>
       <c r="M61" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="N61">
         <v>81</v>
       </c>
       <c r="O61" t="s">
+        <v>373</v>
+      </c>
+      <c r="P61" t="s">
         <v>374</v>
-      </c>
-      <c r="P61" t="s">
-        <v>375</v>
       </c>
       <c r="Z61" t="s">
         <v>126</v>
@@ -8126,10 +8126,10 @@
         <v>39.700000000000003</v>
       </c>
       <c r="O62" t="s">
+        <v>375</v>
+      </c>
+      <c r="P62" t="s">
         <v>376</v>
-      </c>
-      <c r="P62" t="s">
-        <v>377</v>
       </c>
       <c r="Z62" t="s">
         <v>128</v>
@@ -8218,16 +8218,16 @@
         <v>10</v>
       </c>
       <c r="M63" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="N63">
         <v>7.16</v>
       </c>
       <c r="O63" t="s">
+        <v>378</v>
+      </c>
+      <c r="P63" t="s">
         <v>379</v>
-      </c>
-      <c r="P63" t="s">
-        <v>380</v>
       </c>
       <c r="Z63" t="s">
         <v>128</v>
@@ -8326,10 +8326,10 @@
         <v>49.5</v>
       </c>
       <c r="O64" t="s">
+        <v>380</v>
+      </c>
+      <c r="P64" t="s">
         <v>381</v>
-      </c>
-      <c r="P64" t="s">
-        <v>382</v>
       </c>
       <c r="Z64" t="s">
         <v>130</v>
@@ -8428,10 +8428,10 @@
         <v>9.67</v>
       </c>
       <c r="O65" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="P65" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Z65" t="s">
         <v>130</v>
@@ -8778,10 +8778,10 @@
         <v>9.1199999999999992</v>
       </c>
       <c r="O72" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="P72" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="Z72" t="s">
         <v>133</v>
@@ -8858,7 +8858,7 @@
         <v>85</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G73" t="s">
         <v>134</v>
@@ -8880,10 +8880,10 @@
         <v>3.38</v>
       </c>
       <c r="O73" t="s">
+        <v>385</v>
+      </c>
+      <c r="P73" t="s">
         <v>386</v>
-      </c>
-      <c r="P73" t="s">
-        <v>387</v>
       </c>
       <c r="Z73" t="s">
         <v>133</v>
@@ -8972,13 +8972,13 @@
         <v>39</v>
       </c>
       <c r="M74" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="N74">
         <v>420</v>
       </c>
       <c r="O74" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="Z74" t="s">
         <v>136</v>
@@ -9076,7 +9076,7 @@
         <v>1100</v>
       </c>
       <c r="O75" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="Z75" t="s">
         <v>136</v>
@@ -9168,16 +9168,16 @@
         <v>31</v>
       </c>
       <c r="M76" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N76">
         <v>1046</v>
       </c>
       <c r="O76" t="s">
+        <v>389</v>
+      </c>
+      <c r="P76" t="s">
         <v>390</v>
-      </c>
-      <c r="P76" t="s">
-        <v>391</v>
       </c>
       <c r="Q76">
         <v>217</v>
@@ -9278,16 +9278,16 @@
         <v>31</v>
       </c>
       <c r="M77" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="N77">
         <v>676</v>
       </c>
       <c r="O77" t="s">
+        <v>392</v>
+      </c>
+      <c r="P77" t="s">
         <v>393</v>
-      </c>
-      <c r="P77" t="s">
-        <v>394</v>
       </c>
       <c r="Q77">
         <v>173</v>
@@ -9394,10 +9394,10 @@
         <v>94</v>
       </c>
       <c r="O78" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="P78" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="U78">
         <v>2.4</v>
@@ -9502,10 +9502,10 @@
         <v>56</v>
       </c>
       <c r="O79" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="P79" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="U79">
         <v>11</v>
@@ -9591,22 +9591,22 @@
         <v>47</v>
       </c>
       <c r="K80" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L80">
         <v>33</v>
       </c>
       <c r="M80" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="N80">
         <v>1838.17</v>
       </c>
       <c r="O80" t="s">
+        <v>397</v>
+      </c>
+      <c r="P80" t="s">
         <v>398</v>
-      </c>
-      <c r="P80" t="s">
-        <v>399</v>
       </c>
       <c r="Q80">
         <v>479.92168222423498</v>
@@ -9689,22 +9689,22 @@
         <v>56</v>
       </c>
       <c r="K81" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L81">
         <v>33</v>
       </c>
       <c r="M81" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="N81">
         <v>1956.34</v>
       </c>
       <c r="O81" t="s">
+        <v>400</v>
+      </c>
+      <c r="P81" t="s">
         <v>401</v>
-      </c>
-      <c r="P81" t="s">
-        <v>402</v>
       </c>
       <c r="Q81">
         <v>462.79437203361198</v>
@@ -9787,22 +9787,22 @@
         <v>47</v>
       </c>
       <c r="K82" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L82">
         <v>10</v>
       </c>
       <c r="M82" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="N82">
         <v>2674.04</v>
       </c>
       <c r="O82" t="s">
+        <v>403</v>
+      </c>
+      <c r="P82" t="s">
         <v>404</v>
-      </c>
-      <c r="P82" t="s">
-        <v>405</v>
       </c>
       <c r="Q82">
         <v>834.71994308137698</v>
@@ -9885,22 +9885,22 @@
         <v>56</v>
       </c>
       <c r="K83" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L83">
         <v>10</v>
       </c>
       <c r="M83" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="N83">
         <v>3130.08</v>
       </c>
       <c r="O83" t="s">
+        <v>406</v>
+      </c>
+      <c r="P83" t="s">
         <v>407</v>
-      </c>
-      <c r="P83" t="s">
-        <v>408</v>
       </c>
       <c r="Q83">
         <v>1160.95742106222</v>
@@ -9983,22 +9983,22 @@
         <v>47</v>
       </c>
       <c r="K84" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L84">
         <v>29</v>
       </c>
       <c r="M84" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="N84">
         <v>1838.17</v>
       </c>
       <c r="O84" t="s">
+        <v>409</v>
+      </c>
+      <c r="P84" t="s">
         <v>410</v>
-      </c>
-      <c r="P84" t="s">
-        <v>411</v>
       </c>
       <c r="Q84">
         <v>480.79189860124598</v>
@@ -10081,22 +10081,22 @@
         <v>56</v>
       </c>
       <c r="K85" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L85">
         <v>29</v>
       </c>
       <c r="M85" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="N85">
         <v>1956.34</v>
       </c>
       <c r="O85" t="s">
+        <v>412</v>
+      </c>
+      <c r="P85" t="s">
         <v>413</v>
-      </c>
-      <c r="P85" t="s">
-        <v>414</v>
       </c>
       <c r="Q85">
         <v>476.07211632029498</v>
@@ -10191,16 +10191,16 @@
         <v>28</v>
       </c>
       <c r="M86" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="N86">
         <v>125.7</v>
       </c>
       <c r="O86" t="s">
+        <v>415</v>
+      </c>
+      <c r="P86" t="s">
         <v>416</v>
-      </c>
-      <c r="P86" t="s">
-        <v>417</v>
       </c>
       <c r="Q86">
         <v>8.2505731309556491</v>
@@ -10304,10 +10304,10 @@
         <v>28.2</v>
       </c>
       <c r="O87" t="s">
+        <v>417</v>
+      </c>
+      <c r="P87" t="s">
         <v>418</v>
-      </c>
-      <c r="P87" t="s">
-        <v>419</v>
       </c>
       <c r="Q87">
         <v>21.9973312164263</v>
@@ -10402,16 +10402,16 @@
         <v>11</v>
       </c>
       <c r="M88" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="N88">
         <v>13</v>
       </c>
       <c r="O88" t="s">
+        <v>420</v>
+      </c>
+      <c r="P88" t="s">
         <v>421</v>
-      </c>
-      <c r="P88" t="s">
-        <v>422</v>
       </c>
       <c r="Q88">
         <v>3.024</v>
@@ -10503,16 +10503,16 @@
         <v>11</v>
       </c>
       <c r="M89" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="N89">
         <v>6</v>
       </c>
       <c r="O89" t="s">
+        <v>422</v>
+      </c>
+      <c r="P89" t="s">
         <v>423</v>
-      </c>
-      <c r="P89" t="s">
-        <v>424</v>
       </c>
       <c r="Q89">
         <v>1.0369999999999999</v>
@@ -10601,16 +10601,16 @@
         <v>6</v>
       </c>
       <c r="M90" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="N90">
         <v>9</v>
       </c>
       <c r="O90" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="P90" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="Q90">
         <v>1.861</v>
@@ -10699,16 +10699,16 @@
         <v>6</v>
       </c>
       <c r="M91" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="N91">
         <v>6</v>
       </c>
       <c r="O91" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="P91" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="Q91">
         <v>0.78800000000000003</v>
@@ -10801,10 +10801,10 @@
         <v>43</v>
       </c>
       <c r="O92" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="P92" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="W92">
         <v>59</v>
@@ -10896,16 +10896,16 @@
         <v>31</v>
       </c>
       <c r="M93" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="N93">
         <v>303</v>
       </c>
       <c r="O93" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="P93" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Z93" t="s">
         <v>180</v>
@@ -10979,7 +10979,7 @@
         <v>2015</v>
       </c>
       <c r="E94" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F94" t="s">
         <v>47</v>
@@ -11018,7 +11018,7 @@
         <v>2015</v>
       </c>
       <c r="E95" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F95" t="s">
         <v>47</v>
@@ -11057,7 +11057,7 @@
         <v>2015</v>
       </c>
       <c r="E96" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F96" t="s">
         <v>47</v>
@@ -11098,7 +11098,7 @@
         <v>2016</v>
       </c>
       <c r="E97" t="s">
-        <v>182</v>
+        <v>481</v>
       </c>
       <c r="F97" t="s">
         <v>47</v>
@@ -11113,29 +11113,29 @@
         <v>10.3</v>
       </c>
       <c r="Z97" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AB97" t="s">
         <v>66</v>
       </c>
       <c r="AC97" t="s">
+        <v>183</v>
+      </c>
+      <c r="AD97">
+        <v>0</v>
+      </c>
+      <c r="AE97">
+        <v>0</v>
+      </c>
+      <c r="AF97">
+        <v>0</v>
+      </c>
+      <c r="AG97">
+        <v>0</v>
+      </c>
+      <c r="AH97" t="s">
         <v>184</v>
       </c>
-      <c r="AD97">
-        <v>0</v>
-      </c>
-      <c r="AE97">
-        <v>0</v>
-      </c>
-      <c r="AF97">
-        <v>0</v>
-      </c>
-      <c r="AG97">
-        <v>0</v>
-      </c>
-      <c r="AH97" t="s">
-        <v>185</v>
-      </c>
       <c r="AI97" t="s">
         <v>52</v>
       </c>
@@ -11170,7 +11170,7 @@
         <v>1</v>
       </c>
       <c r="AT97" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="98" spans="1:46" x14ac:dyDescent="0.3">
@@ -11178,19 +11178,19 @@
         <v>163</v>
       </c>
       <c r="C98" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D98">
         <v>2011</v>
       </c>
       <c r="E98" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F98" t="s">
         <v>56</v>
       </c>
       <c r="G98" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H98">
         <v>2</v>
@@ -11202,79 +11202,79 @@
         <v>32</v>
       </c>
       <c r="M98" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="N98">
         <v>83.9</v>
       </c>
       <c r="O98" t="s">
+        <v>432</v>
+      </c>
+      <c r="P98" t="s">
         <v>433</v>
-      </c>
-      <c r="P98" t="s">
-        <v>434</v>
       </c>
       <c r="Q98">
         <v>19.11</v>
       </c>
       <c r="Z98" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA98" t="s">
         <v>190</v>
       </c>
-      <c r="AA98" t="s">
+      <c r="AB98" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC98" t="s">
         <v>191</v>
       </c>
-      <c r="AB98" t="s">
-        <v>186</v>
-      </c>
-      <c r="AC98" t="s">
+      <c r="AD98">
+        <v>0</v>
+      </c>
+      <c r="AE98">
+        <v>0</v>
+      </c>
+      <c r="AF98">
+        <v>0</v>
+      </c>
+      <c r="AG98">
+        <v>0</v>
+      </c>
+      <c r="AI98" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ98" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK98" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL98">
+        <v>1</v>
+      </c>
+      <c r="AM98">
+        <v>0</v>
+      </c>
+      <c r="AN98">
+        <v>1</v>
+      </c>
+      <c r="AO98">
+        <v>1</v>
+      </c>
+      <c r="AP98">
+        <v>0</v>
+      </c>
+      <c r="AQ98">
+        <v>1</v>
+      </c>
+      <c r="AR98">
+        <v>0</v>
+      </c>
+      <c r="AS98">
+        <v>1</v>
+      </c>
+      <c r="AT98" t="s">
         <v>192</v>
-      </c>
-      <c r="AD98">
-        <v>0</v>
-      </c>
-      <c r="AE98">
-        <v>0</v>
-      </c>
-      <c r="AF98">
-        <v>0</v>
-      </c>
-      <c r="AG98">
-        <v>0</v>
-      </c>
-      <c r="AI98" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ98" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK98" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL98">
-        <v>1</v>
-      </c>
-      <c r="AM98">
-        <v>0</v>
-      </c>
-      <c r="AN98">
-        <v>1</v>
-      </c>
-      <c r="AO98">
-        <v>1</v>
-      </c>
-      <c r="AP98">
-        <v>0</v>
-      </c>
-      <c r="AQ98">
-        <v>1</v>
-      </c>
-      <c r="AR98">
-        <v>0</v>
-      </c>
-      <c r="AS98">
-        <v>1</v>
-      </c>
-      <c r="AT98" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="99" spans="1:46" x14ac:dyDescent="0.3">
@@ -11282,7 +11282,7 @@
         <v>163</v>
       </c>
       <c r="C99" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D99">
         <v>2011</v>
@@ -11294,7 +11294,7 @@
         <v>47</v>
       </c>
       <c r="G99" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H99">
         <v>1</v>
@@ -11306,32 +11306,32 @@
         <v>32</v>
       </c>
       <c r="M99" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="N99">
         <v>11000</v>
       </c>
       <c r="O99" t="s">
+        <v>434</v>
+      </c>
+      <c r="P99" t="s">
         <v>435</v>
-      </c>
-      <c r="P99" t="s">
-        <v>436</v>
       </c>
       <c r="Q99">
         <v>1955</v>
       </c>
       <c r="Z99" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA99" t="s">
         <v>190</v>
       </c>
-      <c r="AA99" t="s">
+      <c r="AB99" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC99" t="s">
         <v>191</v>
       </c>
-      <c r="AB99" t="s">
-        <v>186</v>
-      </c>
-      <c r="AC99" t="s">
-        <v>192</v>
-      </c>
       <c r="AD99">
         <v>0</v>
       </c>
@@ -11378,7 +11378,7 @@
         <v>1</v>
       </c>
       <c r="AT99" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="100" spans="1:46" x14ac:dyDescent="0.3">
@@ -11386,7 +11386,7 @@
         <v>163</v>
       </c>
       <c r="C100" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D100">
         <v>2011</v>
@@ -11398,7 +11398,7 @@
         <v>56</v>
       </c>
       <c r="G100" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H100">
         <v>2</v>
@@ -11410,79 +11410,79 @@
         <v>19</v>
       </c>
       <c r="M100" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="N100">
         <v>150.6</v>
       </c>
       <c r="O100" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P100" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Q100">
         <v>32.92</v>
       </c>
       <c r="Z100" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA100" t="s">
         <v>190</v>
       </c>
-      <c r="AA100" t="s">
+      <c r="AB100" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC100" t="s">
         <v>191</v>
       </c>
-      <c r="AB100" t="s">
-        <v>186</v>
-      </c>
-      <c r="AC100" t="s">
+      <c r="AD100">
+        <v>0</v>
+      </c>
+      <c r="AE100">
+        <v>0</v>
+      </c>
+      <c r="AF100">
+        <v>0</v>
+      </c>
+      <c r="AG100">
+        <v>0</v>
+      </c>
+      <c r="AI100" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ100" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK100" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL100">
+        <v>1</v>
+      </c>
+      <c r="AM100">
+        <v>0</v>
+      </c>
+      <c r="AN100">
+        <v>1</v>
+      </c>
+      <c r="AO100">
+        <v>1</v>
+      </c>
+      <c r="AP100">
+        <v>0</v>
+      </c>
+      <c r="AQ100">
+        <v>1</v>
+      </c>
+      <c r="AR100">
+        <v>0</v>
+      </c>
+      <c r="AS100">
+        <v>1</v>
+      </c>
+      <c r="AT100" t="s">
         <v>192</v>
-      </c>
-      <c r="AD100">
-        <v>0</v>
-      </c>
-      <c r="AE100">
-        <v>0</v>
-      </c>
-      <c r="AF100">
-        <v>0</v>
-      </c>
-      <c r="AG100">
-        <v>0</v>
-      </c>
-      <c r="AI100" t="s">
-        <v>53</v>
-      </c>
-      <c r="AJ100" t="s">
-        <v>52</v>
-      </c>
-      <c r="AK100" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL100">
-        <v>1</v>
-      </c>
-      <c r="AM100">
-        <v>0</v>
-      </c>
-      <c r="AN100">
-        <v>1</v>
-      </c>
-      <c r="AO100">
-        <v>1</v>
-      </c>
-      <c r="AP100">
-        <v>0</v>
-      </c>
-      <c r="AQ100">
-        <v>1</v>
-      </c>
-      <c r="AR100">
-        <v>0</v>
-      </c>
-      <c r="AS100">
-        <v>1</v>
-      </c>
-      <c r="AT100" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="101" spans="1:46" x14ac:dyDescent="0.3">
@@ -11490,7 +11490,7 @@
         <v>163</v>
       </c>
       <c r="C101" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D101">
         <v>2011</v>
@@ -11502,7 +11502,7 @@
         <v>47</v>
       </c>
       <c r="G101" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H101">
         <v>2</v>
@@ -11514,32 +11514,32 @@
         <v>19</v>
       </c>
       <c r="M101" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="N101">
         <v>6410</v>
       </c>
       <c r="O101" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P101" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="Q101">
         <v>1512</v>
       </c>
       <c r="Z101" t="s">
+        <v>189</v>
+      </c>
+      <c r="AA101" t="s">
         <v>190</v>
       </c>
-      <c r="AA101" t="s">
+      <c r="AB101" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC101" t="s">
         <v>191</v>
       </c>
-      <c r="AB101" t="s">
-        <v>186</v>
-      </c>
-      <c r="AC101" t="s">
-        <v>192</v>
-      </c>
       <c r="AD101">
         <v>0</v>
       </c>
@@ -11586,7 +11586,7 @@
         <v>1</v>
       </c>
       <c r="AT101" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:46" x14ac:dyDescent="0.3">
@@ -11594,19 +11594,19 @@
         <v>163</v>
       </c>
       <c r="C102" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D102">
         <v>2012</v>
       </c>
       <c r="E102" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F102" t="s">
         <v>56</v>
       </c>
       <c r="G102" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H102">
         <v>1</v>
@@ -11628,7 +11628,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="P102" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="Q102">
         <v>812</v>
@@ -11637,7 +11637,7 @@
         <v>129</v>
       </c>
       <c r="AC102" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AD102">
         <v>0</v>
@@ -11690,19 +11690,19 @@
         <v>163</v>
       </c>
       <c r="C103" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D103">
         <v>2012</v>
       </c>
       <c r="E103" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F103" t="s">
         <v>47</v>
       </c>
       <c r="G103" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H103">
         <v>1</v>
@@ -11721,10 +11721,10 @@
         <v>68</v>
       </c>
       <c r="O103" t="s">
+        <v>439</v>
+      </c>
+      <c r="P103" t="s">
         <v>440</v>
-      </c>
-      <c r="P103" t="s">
-        <v>441</v>
       </c>
       <c r="Q103">
         <v>20</v>
@@ -11733,7 +11733,7 @@
         <v>129</v>
       </c>
       <c r="AC103" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AD103">
         <v>0</v>
@@ -11786,19 +11786,19 @@
         <v>163</v>
       </c>
       <c r="C104" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D104">
         <v>2012</v>
       </c>
       <c r="E104" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F104" t="s">
         <v>56</v>
       </c>
       <c r="G104" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H104">
         <v>1</v>
@@ -11817,10 +11817,10 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="O104" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="P104" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q104">
         <v>2.2999999999999998</v>
@@ -11829,7 +11829,7 @@
         <v>109</v>
       </c>
       <c r="AC104" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AD104">
         <v>0</v>
@@ -11882,19 +11882,19 @@
         <v>163</v>
       </c>
       <c r="C105" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D105">
         <v>2012</v>
       </c>
       <c r="E105" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F105" t="s">
         <v>47</v>
       </c>
       <c r="G105" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H105">
         <v>1</v>
@@ -11913,10 +11913,10 @@
         <v>6.5</v>
       </c>
       <c r="O105" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P105" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="Q105">
         <v>2.2000000000000002</v>
@@ -11925,7 +11925,7 @@
         <v>109</v>
       </c>
       <c r="AC105" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AD105">
         <v>0</v>
@@ -11978,19 +11978,19 @@
         <v>163</v>
       </c>
       <c r="C106" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D106">
         <v>2012</v>
       </c>
       <c r="E106" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F106" t="s">
         <v>56</v>
       </c>
       <c r="G106" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H106">
         <v>1</v>
@@ -12012,64 +12012,64 @@
         <v>97</v>
       </c>
       <c r="P106" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="Q106">
         <v>82</v>
       </c>
       <c r="AB106" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC106" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD106">
+        <v>0</v>
+      </c>
+      <c r="AE106">
+        <v>0</v>
+      </c>
+      <c r="AF106">
+        <v>0</v>
+      </c>
+      <c r="AG106">
+        <v>0</v>
+      </c>
+      <c r="AI106" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ106" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK106" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL106">
+        <v>1</v>
+      </c>
+      <c r="AM106">
+        <v>1</v>
+      </c>
+      <c r="AN106">
+        <v>1</v>
+      </c>
+      <c r="AO106">
+        <v>1</v>
+      </c>
+      <c r="AP106">
+        <v>0</v>
+      </c>
+      <c r="AQ106">
+        <v>1</v>
+      </c>
+      <c r="AR106">
+        <v>0</v>
+      </c>
+      <c r="AS106">
+        <v>1</v>
+      </c>
+      <c r="AT106" t="s">
         <v>202</v>
-      </c>
-      <c r="AC106" t="s">
-        <v>198</v>
-      </c>
-      <c r="AD106">
-        <v>0</v>
-      </c>
-      <c r="AE106">
-        <v>0</v>
-      </c>
-      <c r="AF106">
-        <v>0</v>
-      </c>
-      <c r="AG106">
-        <v>0</v>
-      </c>
-      <c r="AI106" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ106" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK106" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL106">
-        <v>1</v>
-      </c>
-      <c r="AM106">
-        <v>1</v>
-      </c>
-      <c r="AN106">
-        <v>1</v>
-      </c>
-      <c r="AO106">
-        <v>1</v>
-      </c>
-      <c r="AP106">
-        <v>0</v>
-      </c>
-      <c r="AQ106">
-        <v>1</v>
-      </c>
-      <c r="AR106">
-        <v>0</v>
-      </c>
-      <c r="AS106">
-        <v>1</v>
-      </c>
-      <c r="AT106" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="107" spans="1:46" x14ac:dyDescent="0.3">
@@ -12077,19 +12077,19 @@
         <v>163</v>
       </c>
       <c r="C107" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D107">
         <v>2012</v>
       </c>
       <c r="E107" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F107" t="s">
         <v>47</v>
       </c>
       <c r="G107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H107">
         <v>1</v>
@@ -12108,67 +12108,67 @@
         <v>35</v>
       </c>
       <c r="O107" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P107" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="Q107">
         <v>8.3000000000000007</v>
       </c>
       <c r="AB107" t="s">
+        <v>201</v>
+      </c>
+      <c r="AC107" t="s">
+        <v>197</v>
+      </c>
+      <c r="AD107">
+        <v>0</v>
+      </c>
+      <c r="AE107">
+        <v>0</v>
+      </c>
+      <c r="AF107">
+        <v>0</v>
+      </c>
+      <c r="AG107">
+        <v>0</v>
+      </c>
+      <c r="AI107" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ107" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK107" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL107">
+        <v>1</v>
+      </c>
+      <c r="AM107">
+        <v>1</v>
+      </c>
+      <c r="AN107">
+        <v>1</v>
+      </c>
+      <c r="AO107">
+        <v>1</v>
+      </c>
+      <c r="AP107">
+        <v>0</v>
+      </c>
+      <c r="AQ107">
+        <v>1</v>
+      </c>
+      <c r="AR107">
+        <v>0</v>
+      </c>
+      <c r="AS107">
+        <v>1</v>
+      </c>
+      <c r="AT107" t="s">
         <v>202</v>
-      </c>
-      <c r="AC107" t="s">
-        <v>198</v>
-      </c>
-      <c r="AD107">
-        <v>0</v>
-      </c>
-      <c r="AE107">
-        <v>0</v>
-      </c>
-      <c r="AF107">
-        <v>0</v>
-      </c>
-      <c r="AG107">
-        <v>0</v>
-      </c>
-      <c r="AI107" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ107" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK107" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL107">
-        <v>1</v>
-      </c>
-      <c r="AM107">
-        <v>1</v>
-      </c>
-      <c r="AN107">
-        <v>1</v>
-      </c>
-      <c r="AO107">
-        <v>1</v>
-      </c>
-      <c r="AP107">
-        <v>0</v>
-      </c>
-      <c r="AQ107">
-        <v>1</v>
-      </c>
-      <c r="AR107">
-        <v>0</v>
-      </c>
-      <c r="AS107">
-        <v>1</v>
-      </c>
-      <c r="AT107" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="108" spans="1:46" x14ac:dyDescent="0.3">
@@ -12176,19 +12176,19 @@
         <v>163</v>
       </c>
       <c r="C108" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D108">
         <v>2012</v>
       </c>
       <c r="E108" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F108" t="s">
         <v>56</v>
       </c>
       <c r="G108" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H108">
         <v>1</v>
@@ -12213,7 +12213,7 @@
         <v>129</v>
       </c>
       <c r="AC108" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AD108">
         <v>0</v>
@@ -12266,19 +12266,19 @@
         <v>163</v>
       </c>
       <c r="C109" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D109">
         <v>2012</v>
       </c>
       <c r="E109" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F109" t="s">
         <v>47</v>
       </c>
       <c r="G109" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H109">
         <v>1</v>
@@ -12297,10 +12297,10 @@
         <v>1.9</v>
       </c>
       <c r="O109" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="P109" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="Q109">
         <v>0.9</v>
@@ -12309,7 +12309,7 @@
         <v>129</v>
       </c>
       <c r="AC109" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AD109">
         <v>0</v>
@@ -12362,22 +12362,22 @@
         <v>163</v>
       </c>
       <c r="C110" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D110">
         <v>2015</v>
       </c>
       <c r="E110" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F110" t="s">
         <v>47</v>
       </c>
       <c r="G110" t="s">
+        <v>206</v>
+      </c>
+      <c r="I110" t="s">
         <v>207</v>
-      </c>
-      <c r="I110" t="s">
-        <v>208</v>
       </c>
       <c r="J110">
         <v>2</v>
@@ -12400,64 +12400,64 @@
         <v>0.59333333333333338</v>
       </c>
       <c r="P110" t="s">
+        <v>445</v>
+      </c>
+      <c r="Z110" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB110" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC110" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD110">
+        <v>0</v>
+      </c>
+      <c r="AE110">
+        <v>0</v>
+      </c>
+      <c r="AF110">
+        <v>0</v>
+      </c>
+      <c r="AG110">
+        <v>0</v>
+      </c>
+      <c r="AI110" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ110" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK110" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL110">
+        <v>1</v>
+      </c>
+      <c r="AM110">
+        <v>1</v>
+      </c>
+      <c r="AN110">
+        <v>1</v>
+      </c>
+      <c r="AO110">
+        <v>1</v>
+      </c>
+      <c r="AP110">
+        <v>0</v>
+      </c>
+      <c r="AQ110">
+        <v>0</v>
+      </c>
+      <c r="AR110">
+        <v>0</v>
+      </c>
+      <c r="AS110">
+        <v>0</v>
+      </c>
+      <c r="AT110" t="s">
         <v>446</v>
-      </c>
-      <c r="Z110" t="s">
-        <v>209</v>
-      </c>
-      <c r="AB110" t="s">
-        <v>210</v>
-      </c>
-      <c r="AC110" t="s">
-        <v>211</v>
-      </c>
-      <c r="AD110">
-        <v>0</v>
-      </c>
-      <c r="AE110">
-        <v>0</v>
-      </c>
-      <c r="AF110">
-        <v>0</v>
-      </c>
-      <c r="AG110">
-        <v>0</v>
-      </c>
-      <c r="AI110" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ110" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK110" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL110">
-        <v>1</v>
-      </c>
-      <c r="AM110">
-        <v>1</v>
-      </c>
-      <c r="AN110">
-        <v>1</v>
-      </c>
-      <c r="AO110">
-        <v>1</v>
-      </c>
-      <c r="AP110">
-        <v>0</v>
-      </c>
-      <c r="AQ110">
-        <v>0</v>
-      </c>
-      <c r="AR110">
-        <v>0</v>
-      </c>
-      <c r="AS110">
-        <v>0</v>
-      </c>
-      <c r="AT110" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="111" spans="1:46" x14ac:dyDescent="0.3">
@@ -12465,13 +12465,13 @@
         <v>163</v>
       </c>
       <c r="C111" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D111">
         <v>2015</v>
       </c>
       <c r="E111" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F111" t="s">
         <v>56</v>
@@ -12480,7 +12480,7 @@
         <v>173</v>
       </c>
       <c r="I111" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K111" t="s">
         <v>167</v>
@@ -12495,19 +12495,19 @@
         <v>44</v>
       </c>
       <c r="O111" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="P111" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="Z111" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB111" t="s">
         <v>209</v>
       </c>
-      <c r="AB111" t="s">
+      <c r="AC111" t="s">
         <v>210</v>
-      </c>
-      <c r="AC111" t="s">
-        <v>211</v>
       </c>
       <c r="AD111">
         <v>0</v>
@@ -12560,22 +12560,22 @@
         <v>163</v>
       </c>
       <c r="C112" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D112">
         <v>2015</v>
       </c>
       <c r="E112" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F112" t="s">
         <v>47</v>
       </c>
       <c r="G112" t="s">
+        <v>206</v>
+      </c>
+      <c r="I112" t="s">
         <v>207</v>
-      </c>
-      <c r="I112" t="s">
-        <v>208</v>
       </c>
       <c r="J112">
         <v>2</v>
@@ -12598,16 +12598,16 @@
         <v>0.59333333333333338</v>
       </c>
       <c r="P112" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="Z112" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB112" t="s">
         <v>107</v>
       </c>
       <c r="AC112" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AD112">
         <v>0</v>
@@ -12660,13 +12660,13 @@
         <v>163</v>
       </c>
       <c r="C113" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D113">
         <v>2015</v>
       </c>
       <c r="E113" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F113" t="s">
         <v>56</v>
@@ -12675,7 +12675,7 @@
         <v>173</v>
       </c>
       <c r="I113" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J113">
         <v>2</v>
@@ -12695,16 +12695,16 @@
         <v>0.27333333333333332</v>
       </c>
       <c r="P113" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="Z113" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB113" t="s">
         <v>107</v>
       </c>
       <c r="AC113" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AD113">
         <v>0</v>
@@ -12752,7 +12752,7 @@
         <v>0</v>
       </c>
       <c r="AT113" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="114" spans="1:46" x14ac:dyDescent="0.3">
@@ -12760,22 +12760,22 @@
         <v>163</v>
       </c>
       <c r="C114" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D114">
         <v>2015</v>
       </c>
       <c r="E114" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F114" t="s">
         <v>47</v>
       </c>
       <c r="G114" t="s">
+        <v>206</v>
+      </c>
+      <c r="I114" t="s">
         <v>207</v>
-      </c>
-      <c r="I114" t="s">
-        <v>208</v>
       </c>
       <c r="J114">
         <v>2</v>
@@ -12798,16 +12798,16 @@
         <v>0.59333333333333338</v>
       </c>
       <c r="P114" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="Z114" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AB114" t="s">
         <v>129</v>
       </c>
       <c r="AC114" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AD114">
         <v>0</v>
@@ -12860,13 +12860,13 @@
         <v>163</v>
       </c>
       <c r="C115" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D115">
         <v>2015</v>
       </c>
       <c r="E115" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F115" t="s">
         <v>56</v>
@@ -12875,7 +12875,7 @@
         <v>173</v>
       </c>
       <c r="I115" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J115">
         <v>2</v>
@@ -12898,16 +12898,16 @@
         <v>0.27333333333333332</v>
       </c>
       <c r="P115" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Z115" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AB115" t="s">
         <v>129</v>
       </c>
       <c r="AC115" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AD115">
         <v>0</v>
@@ -12960,22 +12960,22 @@
         <v>163</v>
       </c>
       <c r="C116" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D116">
         <v>2015</v>
       </c>
       <c r="E116" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F116" t="s">
         <v>47</v>
       </c>
       <c r="G116" t="s">
+        <v>206</v>
+      </c>
+      <c r="I116" t="s">
         <v>207</v>
-      </c>
-      <c r="I116" t="s">
-        <v>208</v>
       </c>
       <c r="J116">
         <v>2</v>
@@ -12998,16 +12998,16 @@
         <v>0.59333333333333338</v>
       </c>
       <c r="P116" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="Z116" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB116" t="s">
         <v>209</v>
       </c>
-      <c r="AB116" t="s">
+      <c r="AC116" t="s">
         <v>210</v>
-      </c>
-      <c r="AC116" t="s">
-        <v>211</v>
       </c>
       <c r="AD116">
         <v>0</v>
@@ -13060,22 +13060,22 @@
         <v>163</v>
       </c>
       <c r="C117" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D117">
         <v>2015</v>
       </c>
       <c r="E117" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F117" t="s">
         <v>47</v>
       </c>
       <c r="G117" t="s">
+        <v>206</v>
+      </c>
+      <c r="I117" t="s">
         <v>207</v>
-      </c>
-      <c r="I117" t="s">
-        <v>208</v>
       </c>
       <c r="J117">
         <v>2</v>
@@ -13098,16 +13098,16 @@
         <v>0.59333333333333338</v>
       </c>
       <c r="P117" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="Z117" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB117" t="s">
         <v>107</v>
       </c>
       <c r="AC117" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AD117">
         <v>0</v>
@@ -13160,13 +13160,13 @@
         <v>163</v>
       </c>
       <c r="C118" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D118">
         <v>2015</v>
       </c>
       <c r="E118" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F118" t="s">
         <v>56</v>
@@ -13175,7 +13175,7 @@
         <v>173</v>
       </c>
       <c r="I118" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J118">
         <v>2</v>
@@ -13201,13 +13201,13 @@
         <v>5.2</v>
       </c>
       <c r="Z118" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AB118" t="s">
         <v>107</v>
       </c>
       <c r="AC118" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AD118">
         <v>0</v>
@@ -13260,22 +13260,22 @@
         <v>163</v>
       </c>
       <c r="C119" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D119">
         <v>2015</v>
       </c>
       <c r="E119" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F119" t="s">
         <v>47</v>
       </c>
       <c r="G119" t="s">
+        <v>206</v>
+      </c>
+      <c r="I119" t="s">
         <v>207</v>
-      </c>
-      <c r="I119" t="s">
-        <v>208</v>
       </c>
       <c r="J119">
         <v>2</v>
@@ -13298,16 +13298,16 @@
         <v>0.59333333333333338</v>
       </c>
       <c r="P119" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="Z119" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AB119" t="s">
         <v>129</v>
       </c>
       <c r="AC119" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="AD119">
         <v>0</v>
@@ -13360,13 +13360,13 @@
         <v>163</v>
       </c>
       <c r="C120" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D120">
         <v>2015</v>
       </c>
       <c r="E120" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F120" t="s">
         <v>56</v>
@@ -13375,7 +13375,7 @@
         <v>173</v>
       </c>
       <c r="I120" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J120">
         <v>4</v>
@@ -13408,13 +13408,13 @@
         <v>163</v>
       </c>
       <c r="C121" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D121">
         <v>2015</v>
       </c>
       <c r="E121" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F121" t="s">
         <v>56</v>
@@ -13423,7 +13423,7 @@
         <v>173</v>
       </c>
       <c r="I121" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J121">
         <v>4</v>
@@ -13456,19 +13456,19 @@
         <v>163</v>
       </c>
       <c r="C122" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D122">
         <v>2016</v>
       </c>
       <c r="E122" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F122" t="s">
         <v>47</v>
       </c>
       <c r="I122" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K122" t="s">
         <v>167</v>
@@ -13483,10 +13483,10 @@
         <v>105.12</v>
       </c>
       <c r="P122" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AB122" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AC122" t="s">
         <v>67</v>
@@ -13504,43 +13504,43 @@
         <v>0</v>
       </c>
       <c r="AH122" t="s">
+        <v>226</v>
+      </c>
+      <c r="AI122" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ122" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK122" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL122">
+        <v>1</v>
+      </c>
+      <c r="AM122">
+        <v>1</v>
+      </c>
+      <c r="AN122">
+        <v>1</v>
+      </c>
+      <c r="AO122">
+        <v>1</v>
+      </c>
+      <c r="AP122">
+        <v>0</v>
+      </c>
+      <c r="AQ122">
+        <v>1</v>
+      </c>
+      <c r="AR122">
+        <v>0</v>
+      </c>
+      <c r="AS122">
+        <v>1</v>
+      </c>
+      <c r="AT122" t="s">
         <v>227</v>
-      </c>
-      <c r="AI122" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ122" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK122" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL122">
-        <v>1</v>
-      </c>
-      <c r="AM122">
-        <v>1</v>
-      </c>
-      <c r="AN122">
-        <v>1</v>
-      </c>
-      <c r="AO122">
-        <v>1</v>
-      </c>
-      <c r="AP122">
-        <v>0</v>
-      </c>
-      <c r="AQ122">
-        <v>1</v>
-      </c>
-      <c r="AR122">
-        <v>0</v>
-      </c>
-      <c r="AS122">
-        <v>1</v>
-      </c>
-      <c r="AT122" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="123" spans="1:46" x14ac:dyDescent="0.3">
@@ -13548,19 +13548,19 @@
         <v>163</v>
       </c>
       <c r="C123" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D123">
         <v>2016</v>
       </c>
       <c r="E123" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F123" t="s">
         <v>56</v>
       </c>
       <c r="I123" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K123" t="s">
         <v>167</v>
@@ -13569,16 +13569,16 @@
         <v>10</v>
       </c>
       <c r="M123" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="N123">
         <v>1.72</v>
       </c>
       <c r="P123" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AB123" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AC123" t="s">
         <v>67</v>
@@ -13596,7 +13596,7 @@
         <v>0</v>
       </c>
       <c r="AH123" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AI123" t="s">
         <v>52</v>
@@ -13637,19 +13637,19 @@
         <v>163</v>
       </c>
       <c r="C124" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D124">
         <v>2016</v>
       </c>
       <c r="E124" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F124" t="s">
         <v>47</v>
       </c>
       <c r="I124" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K124" t="s">
         <v>167</v>
@@ -13658,16 +13658,16 @@
         <v>10</v>
       </c>
       <c r="M124" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="N124">
         <v>47.7</v>
       </c>
       <c r="P124" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="AB124" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AC124" t="s">
         <v>67</v>
@@ -13685,43 +13685,43 @@
         <v>0</v>
       </c>
       <c r="AH124" t="s">
+        <v>226</v>
+      </c>
+      <c r="AI124" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ124" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK124" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL124">
+        <v>1</v>
+      </c>
+      <c r="AM124">
+        <v>1</v>
+      </c>
+      <c r="AN124">
+        <v>1</v>
+      </c>
+      <c r="AO124">
+        <v>1</v>
+      </c>
+      <c r="AP124">
+        <v>0</v>
+      </c>
+      <c r="AQ124">
+        <v>1</v>
+      </c>
+      <c r="AR124">
+        <v>0</v>
+      </c>
+      <c r="AS124">
+        <v>1</v>
+      </c>
+      <c r="AT124" t="s">
         <v>227</v>
-      </c>
-      <c r="AI124" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ124" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK124" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL124">
-        <v>1</v>
-      </c>
-      <c r="AM124">
-        <v>1</v>
-      </c>
-      <c r="AN124">
-        <v>1</v>
-      </c>
-      <c r="AO124">
-        <v>1</v>
-      </c>
-      <c r="AP124">
-        <v>0</v>
-      </c>
-      <c r="AQ124">
-        <v>1</v>
-      </c>
-      <c r="AR124">
-        <v>0</v>
-      </c>
-      <c r="AS124">
-        <v>1</v>
-      </c>
-      <c r="AT124" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="125" spans="1:46" x14ac:dyDescent="0.3">
@@ -13729,19 +13729,19 @@
         <v>163</v>
       </c>
       <c r="C125" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D125">
         <v>2016</v>
       </c>
       <c r="E125" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F125" t="s">
         <v>56</v>
       </c>
       <c r="I125" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K125" t="s">
         <v>167</v>
@@ -13750,16 +13750,16 @@
         <v>10</v>
       </c>
       <c r="M125" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="N125">
         <v>11.03</v>
       </c>
       <c r="P125" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="AB125" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AC125" t="s">
         <v>67</v>
@@ -13777,7 +13777,7 @@
         <v>0</v>
       </c>
       <c r="AH125" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AI125" t="s">
         <v>52</v>
@@ -13818,19 +13818,19 @@
         <v>163</v>
       </c>
       <c r="C126" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D126">
         <v>2016</v>
       </c>
       <c r="E126" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F126" t="s">
         <v>47</v>
       </c>
       <c r="I126" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K126" t="s">
         <v>167</v>
@@ -13839,16 +13839,16 @@
         <v>10</v>
       </c>
       <c r="M126" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="N126">
         <v>60.35</v>
       </c>
       <c r="P126" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="AB126" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AC126" t="s">
         <v>67</v>
@@ -13866,43 +13866,43 @@
         <v>0</v>
       </c>
       <c r="AH126" t="s">
+        <v>226</v>
+      </c>
+      <c r="AI126" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ126" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK126" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL126">
+        <v>1</v>
+      </c>
+      <c r="AM126">
+        <v>1</v>
+      </c>
+      <c r="AN126">
+        <v>1</v>
+      </c>
+      <c r="AO126">
+        <v>1</v>
+      </c>
+      <c r="AP126">
+        <v>0</v>
+      </c>
+      <c r="AQ126">
+        <v>1</v>
+      </c>
+      <c r="AR126">
+        <v>0</v>
+      </c>
+      <c r="AS126">
+        <v>1</v>
+      </c>
+      <c r="AT126" t="s">
         <v>227</v>
-      </c>
-      <c r="AI126" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ126" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK126" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL126">
-        <v>1</v>
-      </c>
-      <c r="AM126">
-        <v>1</v>
-      </c>
-      <c r="AN126">
-        <v>1</v>
-      </c>
-      <c r="AO126">
-        <v>1</v>
-      </c>
-      <c r="AP126">
-        <v>0</v>
-      </c>
-      <c r="AQ126">
-        <v>1</v>
-      </c>
-      <c r="AR126">
-        <v>0</v>
-      </c>
-      <c r="AS126">
-        <v>1</v>
-      </c>
-      <c r="AT126" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="127" spans="1:46" x14ac:dyDescent="0.3">
@@ -13910,19 +13910,19 @@
         <v>163</v>
       </c>
       <c r="C127" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D127">
         <v>2016</v>
       </c>
       <c r="E127" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F127" t="s">
         <v>56</v>
       </c>
       <c r="I127" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="K127" t="s">
         <v>167</v>
@@ -13931,16 +13931,16 @@
         <v>10</v>
       </c>
       <c r="M127" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="N127">
         <v>6.01</v>
       </c>
       <c r="P127" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AB127" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AC127" t="s">
         <v>67</v>
@@ -13958,7 +13958,7 @@
         <v>0</v>
       </c>
       <c r="AH127" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AI127" t="s">
         <v>52</v>
@@ -13999,19 +13999,19 @@
         <v>163</v>
       </c>
       <c r="C128" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D128">
         <v>2016</v>
       </c>
       <c r="E128" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F128" t="s">
         <v>47</v>
       </c>
       <c r="I128" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K128" t="s">
         <v>167</v>
@@ -14026,10 +14026,10 @@
         <v>11</v>
       </c>
       <c r="P128" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AB128" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="AC128" t="s">
         <v>67</v>
@@ -14047,43 +14047,43 @@
         <v>0</v>
       </c>
       <c r="AH128" t="s">
+        <v>226</v>
+      </c>
+      <c r="AI128" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ128" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK128" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL128">
+        <v>1</v>
+      </c>
+      <c r="AM128">
+        <v>1</v>
+      </c>
+      <c r="AN128">
+        <v>1</v>
+      </c>
+      <c r="AO128">
+        <v>1</v>
+      </c>
+      <c r="AP128">
+        <v>0</v>
+      </c>
+      <c r="AQ128">
+        <v>1</v>
+      </c>
+      <c r="AR128">
+        <v>0</v>
+      </c>
+      <c r="AS128">
+        <v>1</v>
+      </c>
+      <c r="AT128" t="s">
         <v>227</v>
-      </c>
-      <c r="AI128" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ128" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK128" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL128">
-        <v>1</v>
-      </c>
-      <c r="AM128">
-        <v>1</v>
-      </c>
-      <c r="AN128">
-        <v>1</v>
-      </c>
-      <c r="AO128">
-        <v>1</v>
-      </c>
-      <c r="AP128">
-        <v>0</v>
-      </c>
-      <c r="AQ128">
-        <v>1</v>
-      </c>
-      <c r="AR128">
-        <v>0</v>
-      </c>
-      <c r="AS128">
-        <v>1</v>
-      </c>
-      <c r="AT128" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="129" spans="1:46" x14ac:dyDescent="0.3">
@@ -14091,19 +14091,19 @@
         <v>163</v>
       </c>
       <c r="C129" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D129">
         <v>2016</v>
       </c>
       <c r="E129" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F129" t="s">
         <v>47</v>
       </c>
       <c r="G129" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H129">
         <v>1</v>
@@ -14122,16 +14122,16 @@
         <v>137</v>
       </c>
       <c r="O129" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="P129" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AA129" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AB129" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AC129" t="s">
         <v>116</v>
@@ -14149,7 +14149,7 @@
         <v>0</v>
       </c>
       <c r="AH129" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AI129" t="s">
         <v>52</v>
@@ -14190,19 +14190,19 @@
         <v>163</v>
       </c>
       <c r="C130" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D130">
         <v>2016</v>
       </c>
       <c r="E130" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F130" t="s">
         <v>56</v>
       </c>
       <c r="G130" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H130">
         <v>1</v>
@@ -14221,16 +14221,16 @@
         <v>346</v>
       </c>
       <c r="O130" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="P130" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="AA130" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AB130" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AC130" t="s">
         <v>116</v>
@@ -14248,7 +14248,7 @@
         <v>0</v>
       </c>
       <c r="AH130" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AI130" t="s">
         <v>52</v>
@@ -14289,19 +14289,19 @@
         <v>163</v>
       </c>
       <c r="C131" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D131">
         <v>2016</v>
       </c>
       <c r="E131" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F131" t="s">
         <v>47</v>
       </c>
       <c r="G131" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H131">
         <v>3</v>
@@ -14328,10 +14328,10 @@
         <v>6.666666666666667</v>
       </c>
       <c r="AA131" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AB131" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AC131" t="s">
         <v>116</v>
@@ -14349,7 +14349,7 @@
         <v>0</v>
       </c>
       <c r="AH131" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AI131" t="s">
         <v>52</v>
@@ -14390,19 +14390,19 @@
         <v>163</v>
       </c>
       <c r="C132" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D132">
         <v>2016</v>
       </c>
       <c r="E132" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F132" t="s">
         <v>56</v>
       </c>
       <c r="G132" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H132">
         <v>3</v>
@@ -14429,10 +14429,10 @@
         <v>16.666666666666668</v>
       </c>
       <c r="AA132" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AB132" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AC132" t="s">
         <v>116</v>
@@ -14450,7 +14450,7 @@
         <v>0</v>
       </c>
       <c r="AH132" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AI132" t="s">
         <v>52</v>
@@ -14491,19 +14491,19 @@
         <v>163</v>
       </c>
       <c r="C133" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D133">
         <v>2016</v>
       </c>
       <c r="E133" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F133" t="s">
         <v>47</v>
       </c>
       <c r="G133" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H133">
         <v>3</v>
@@ -14530,10 +14530,10 @@
         <v>6.666666666666667</v>
       </c>
       <c r="AA133" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AB133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AC133" t="s">
         <v>116</v>
@@ -14551,7 +14551,7 @@
         <v>0</v>
       </c>
       <c r="AH133" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AI133" t="s">
         <v>52</v>
@@ -14592,19 +14592,19 @@
         <v>163</v>
       </c>
       <c r="C134" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D134">
         <v>2016</v>
       </c>
       <c r="E134" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F134" t="s">
         <v>56</v>
       </c>
       <c r="G134" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H134">
         <v>3</v>
@@ -14631,10 +14631,10 @@
         <v>16.666666666666668</v>
       </c>
       <c r="AA134" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AB134" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AC134" t="s">
         <v>116</v>
@@ -14652,7 +14652,7 @@
         <v>0</v>
       </c>
       <c r="AH134" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AI134" t="s">
         <v>52</v>
@@ -14693,13 +14693,13 @@
         <v>163</v>
       </c>
       <c r="C135" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D135">
         <v>2011</v>
       </c>
       <c r="E135" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F135" t="s">
         <v>47</v>
@@ -14717,22 +14717,22 @@
         <v>7</v>
       </c>
       <c r="M135" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="N135">
         <v>8.56</v>
       </c>
       <c r="O135" t="s">
+        <v>469</v>
+      </c>
+      <c r="P135" t="s">
         <v>470</v>
-      </c>
-      <c r="P135" t="s">
-        <v>471</v>
       </c>
       <c r="Q135">
         <v>2.794</v>
       </c>
       <c r="AB135" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AC135" t="s">
         <v>81</v>
@@ -14788,19 +14788,19 @@
         <v>163</v>
       </c>
       <c r="C136" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D136">
         <v>2011</v>
       </c>
       <c r="E136" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F136" t="s">
         <v>56</v>
       </c>
       <c r="G136" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="I136">
         <v>2.4E-2</v>
@@ -14812,22 +14812,22 @@
         <v>7</v>
       </c>
       <c r="M136" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N136">
         <v>8.81</v>
       </c>
       <c r="O136" t="s">
+        <v>472</v>
+      </c>
+      <c r="P136" t="s">
         <v>473</v>
-      </c>
-      <c r="P136" t="s">
-        <v>474</v>
       </c>
       <c r="Q136">
         <v>3.4420000000000002</v>
       </c>
       <c r="AB136" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="AC136" t="s">
         <v>81</v>
@@ -14883,13 +14883,13 @@
         <v>163</v>
       </c>
       <c r="C137" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D137">
         <v>2015</v>
       </c>
       <c r="E137" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F137" t="s">
         <v>47</v>
@@ -14923,13 +14923,13 @@
         <v>163</v>
       </c>
       <c r="C138" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D138">
         <v>2015</v>
       </c>
       <c r="E138" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F138" t="s">
         <v>56</v>
@@ -14964,13 +14964,13 @@
         <v>163</v>
       </c>
       <c r="C139" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D139">
         <v>2015</v>
       </c>
       <c r="E139" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F139" t="s">
         <v>47</v>
@@ -15004,13 +15004,13 @@
         <v>163</v>
       </c>
       <c r="C140" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D140">
         <v>2015</v>
       </c>
       <c r="E140" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F140" t="s">
         <v>56</v>
@@ -15044,7 +15044,7 @@
         <v>163</v>
       </c>
       <c r="C141" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D141">
         <v>2016</v>
@@ -15071,17 +15071,17 @@
         <v>56</v>
       </c>
       <c r="O141" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AA141" t="s">
+        <v>244</v>
+      </c>
+      <c r="AB141" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC141" t="s">
         <v>245</v>
       </c>
-      <c r="AB141" t="s">
-        <v>186</v>
-      </c>
-      <c r="AC141" t="s">
-        <v>246</v>
-      </c>
       <c r="AD141">
         <v>0</v>
       </c>
@@ -15128,7 +15128,7 @@
         <v>1</v>
       </c>
       <c r="AT141" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="142" spans="1:46" x14ac:dyDescent="0.3">
@@ -15136,7 +15136,7 @@
         <v>163</v>
       </c>
       <c r="C142" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D142">
         <v>2016</v>
@@ -15167,16 +15167,16 @@
         <v>27.5</v>
       </c>
       <c r="O142" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AA142" t="s">
+        <v>244</v>
+      </c>
+      <c r="AB142" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC142" t="s">
         <v>245</v>
-      </c>
-      <c r="AB142" t="s">
-        <v>186</v>
-      </c>
-      <c r="AC142" t="s">
-        <v>246</v>
       </c>
       <c r="AD142">
         <v>0</v>
@@ -15239,15 +15239,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100175F8EE2D16CCF4E9795DBA2E0366580" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a0e36aa337ceae7f1d93f3efc48c3ea9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e6ae508a-59c9-42bb-b4fe-819888132927" xmlns:ns4="7d98c609-804a-400c-9f9b-45f6e3b4e0b0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="376aea29d8ef60d7b2126687d24b7c91" ns3:_="" ns4:_="">
     <xsd:import namespace="e6ae508a-59c9-42bb-b4fe-819888132927"/>
@@ -15456,6 +15447,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{619936EC-EF42-4CC2-B464-377D7CE891A9}">
   <ds:schemaRefs>
@@ -15474,14 +15474,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A602FC1-DACC-4B1D-A27E-1705833C36F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ECAB6FE-ED10-48D6-B2FD-BD0018793311}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15498,4 +15490,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A602FC1-DACC-4B1D-A27E-1705833C36F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>